<commit_message>
finished making ExcelWriter tests for paired data and time series
created additional methods for writing paired data

changed signatures of some methods

added null reference check in row count and column count methods
</commit_message>
<xml_diff>
--- a/DSSExcelTests/test-files/write-test-existing.xlsx
+++ b/DSSExcelTests/test-files/write-test-existing.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fileVersion appName="SpreadsheetGear 8.4.3.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -9,21 +9,188 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="40001"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>1Day</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Date/Time</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -49,22 +216,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -111,7 +269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -146,7 +304,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -245,21 +403,18 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -321,22 +476,161 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row>
+      <c t="s">
+        <v>13</v>
+      </c>
+      <c t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>0</v>
+      </c>
+      <c t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>6</v>
+      </c>
+      <c t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>14</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>2</v>
+      </c>
+      <c t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row>
+      <c t="s">
+        <v>9</v>
+      </c>
+      <c t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row>
+      <c s="1">
+        <v>43831</v>
+      </c>
+      <c>
+        <v>0</v>
+      </c>
+    </row>
+    <row>
+      <c s="1">
+        <v>43832</v>
+      </c>
+      <c>
+        <v>2</v>
+      </c>
+    </row>
+    <row>
+      <c s="1">
+        <v>43833</v>
+      </c>
+      <c>
+        <v>4</v>
+      </c>
+    </row>
+    <row>
+      <c s="1">
+        <v>43834</v>
+      </c>
+      <c>
+        <v>6</v>
+      </c>
+    </row>
+    <row>
+      <c s="1">
+        <v>43835</v>
+      </c>
+      <c>
+        <v>8</v>
+      </c>
+    </row>
+    <row>
+      <c s="1">
+        <v>43836</v>
+      </c>
+      <c>
+        <v>10</v>
+      </c>
+    </row>
+    <row>
+      <c s="1">
+        <v>43837</v>
+      </c>
+      <c>
+        <v>12</v>
+      </c>
+    </row>
+    <row>
+      <c s="1">
+        <v>43838</v>
+      </c>
+      <c>
+        <v>14</v>
+      </c>
+    </row>
+    <row>
+      <c s="1">
+        <v>43839</v>
+      </c>
+      <c>
+        <v>16</v>
+      </c>
+    </row>
+    <row>
+      <c s="1">
+        <v>43840</v>
+      </c>
+      <c>
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>